<commit_message>
rename Collection to CRF in tabs
</commit_message>
<xml_diff>
--- a/curation/draft/crf/crf_specialization_AE.xlsx
+++ b/curation/draft/crf/crf_specialization_AE.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\collection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\crf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A95C79-1FD2-4B5E-8F37-7813C5DB60BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09D8C9D-9C96-4859-9FF3-F21D7D2BC1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="915" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Collection_AE" sheetId="1" r:id="rId1"/>
+    <sheet name="CRF_AE" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_AE!$A$1:$AK$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CRF_AE!$A$1:$AK$34</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>

</xml_diff>